<commit_message>
preparando modelos colbert para 10k
</commit_message>
<xml_diff>
--- a/colbert/output/Results_colbert_avg_body_split_bm25_extraQuestions.xlsx
+++ b/colbert/output/Results_colbert_avg_body_split_bm25_extraQuestions.xlsx
@@ -1002,11 +1002,11 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>109439</v>
+        <v>84797</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>berry  good sandwich spread</t>
+          <t>love is in the air  beef fondue   sauces</t>
         </is>
       </c>
     </row>
@@ -1027,11 +1027,11 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>84797</v>
+        <v>109439</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>love is in the air  beef fondue   sauces</t>
+          <t>berry  good sandwich spread</t>
         </is>
       </c>
     </row>
@@ -1052,11 +1052,11 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>62368</v>
+        <v>42522</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>the best  chocolate chip cheesecake ever</t>
+          <t>the man s  taco dip</t>
         </is>
       </c>
     </row>
@@ -1077,11 +1077,11 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>42522</v>
+        <v>62368</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>the man s  taco dip</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -1252,11 +1252,11 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>93249</v>
+        <v>76808</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>grilled  ranch bread</t>
+          <t>cream  of spinach soup</t>
         </is>
       </c>
     </row>
@@ -1277,11 +1277,11 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>76808</v>
+        <v>93249</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>cream  of spinach soup</t>
+          <t>grilled  ranch bread</t>
         </is>
       </c>
     </row>
@@ -1327,11 +1327,11 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>42522</v>
+        <v>112959</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>the man s  taco dip</t>
+          <t>sour cream  avocado dip  vegan</t>
         </is>
       </c>
     </row>
@@ -1377,11 +1377,11 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>24701</v>
+        <v>76808</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>cream  of spinach soup  vegan</t>
+          <t>cream  of spinach soup</t>
         </is>
       </c>
     </row>
@@ -1402,11 +1402,11 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>76808</v>
+        <v>24701</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>cream  of spinach soup</t>
+          <t>cream  of spinach soup  vegan</t>
         </is>
       </c>
     </row>
@@ -1427,11 +1427,11 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>93249</v>
+        <v>74805</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>grilled  ranch bread</t>
+          <t>never weep  whipped cream</t>
         </is>
       </c>
     </row>
@@ -1452,11 +1452,11 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>74805</v>
+        <v>93249</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>never weep  whipped cream</t>
+          <t>grilled  ranch bread</t>
         </is>
       </c>
     </row>
@@ -2402,11 +2402,11 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>32271</v>
+        <v>62368</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>one pot  brownies</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -2427,11 +2427,11 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>62368</v>
+        <v>32271</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>the best  chocolate chip cheesecake ever</t>
+          <t>one pot  brownies</t>
         </is>
       </c>
     </row>
@@ -3352,11 +3352,11 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>19208</v>
+        <v>63593</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>red hot  applesauce</t>
+          <t>more  more    apple pear jigglers</t>
         </is>
       </c>
     </row>
@@ -3377,11 +3377,11 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>63593</v>
+        <v>19208</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>more  more    apple pear jigglers</t>
+          <t>red hot  applesauce</t>
         </is>
       </c>
     </row>
@@ -4352,11 +4352,11 @@
         </is>
       </c>
       <c r="D157" t="n">
-        <v>39363</v>
+        <v>83062</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>the best  banana bread  or muffins</t>
+          <t>spicy  banana bread</t>
         </is>
       </c>
     </row>
@@ -4377,11 +4377,11 @@
         </is>
       </c>
       <c r="D158" t="n">
-        <v>83062</v>
+        <v>39363</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>spicy  banana bread</t>
+          <t>the best  banana bread  or muffins</t>
         </is>
       </c>
     </row>
@@ -5077,11 +5077,11 @@
         </is>
       </c>
       <c r="D186" t="n">
-        <v>47366</v>
+        <v>38276</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>forgotten  minestrone</t>
+          <t>now and later  vegetarian empanadas</t>
         </is>
       </c>
     </row>
@@ -5277,11 +5277,11 @@
         </is>
       </c>
       <c r="D194" t="n">
-        <v>35964</v>
+        <v>62368</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>rich  hot fudge cake</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -5302,11 +5302,11 @@
         </is>
       </c>
       <c r="D195" t="n">
-        <v>24701</v>
+        <v>35964</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>cream  of spinach soup  vegan</t>
+          <t>rich  hot fudge cake</t>
         </is>
       </c>
     </row>
@@ -5327,11 +5327,11 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>112959</v>
+        <v>24701</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>sour cream  avocado dip  vegan</t>
+          <t>cream  of spinach soup  vegan</t>
         </is>
       </c>
     </row>
@@ -5427,11 +5427,11 @@
         </is>
       </c>
       <c r="D200" t="n">
-        <v>90921</v>
+        <v>39363</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>i stole the idea from mirj  sesame noodles</t>
+          <t>the best  banana bread  or muffins</t>
         </is>
       </c>
     </row>
@@ -5452,11 +5452,11 @@
         </is>
       </c>
       <c r="D201" t="n">
-        <v>24701</v>
+        <v>62368</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>cream  of spinach soup  vegan</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -6252,11 +6252,11 @@
         </is>
       </c>
       <c r="D233" t="n">
-        <v>32271</v>
+        <v>83025</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>one pot  brownies</t>
+          <t>jeanne s style  birthday cake</t>
         </is>
       </c>
     </row>
@@ -6277,11 +6277,11 @@
         </is>
       </c>
       <c r="D234" t="n">
-        <v>58651</v>
+        <v>35964</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>turtle  squares</t>
+          <t>rich  hot fudge cake</t>
         </is>
       </c>
     </row>
@@ -6302,11 +6302,11 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>83025</v>
+        <v>32271</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>jeanne s style  birthday cake</t>
+          <t>one pot  brownies</t>
         </is>
       </c>
     </row>
@@ -6327,11 +6327,11 @@
         </is>
       </c>
       <c r="D236" t="n">
-        <v>35964</v>
+        <v>58651</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>rich  hot fudge cake</t>
+          <t>turtle  squares</t>
         </is>
       </c>
     </row>
@@ -6452,11 +6452,11 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>71635</v>
+        <v>52804</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>no bake  cookie crumble cheesecake</t>
+          <t>jiffy  extra moist carrot cake</t>
         </is>
       </c>
     </row>
@@ -7002,11 +7002,11 @@
         </is>
       </c>
       <c r="D263" t="n">
-        <v>39363</v>
+        <v>62368</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>the best  banana bread  or muffins</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -7027,11 +7027,11 @@
         </is>
       </c>
       <c r="D264" t="n">
-        <v>62368</v>
+        <v>39363</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>the best  chocolate chip cheesecake ever</t>
+          <t>the best  banana bread  or muffins</t>
         </is>
       </c>
     </row>
@@ -7277,11 +7277,11 @@
         </is>
       </c>
       <c r="D274" t="n">
-        <v>71635</v>
+        <v>62368</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>no bake  cookie crumble cheesecake</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -7302,11 +7302,11 @@
         </is>
       </c>
       <c r="D275" t="n">
-        <v>49262</v>
+        <v>71635</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>easiest ever  hollandaise sauce</t>
+          <t>no bake  cookie crumble cheesecake</t>
         </is>
       </c>
     </row>
@@ -7327,11 +7327,11 @@
         </is>
       </c>
       <c r="D276" t="n">
-        <v>62368</v>
+        <v>49262</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>the best  chocolate chip cheesecake ever</t>
+          <t>easiest ever  hollandaise sauce</t>
         </is>
       </c>
     </row>
@@ -8077,11 +8077,11 @@
         </is>
       </c>
       <c r="D306" t="n">
-        <v>42570</v>
+        <v>41756</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>pick me up  party chicken kabobs</t>
+          <t>souper  easy sweet   sour meatballs</t>
         </is>
       </c>
     </row>
@@ -9027,11 +9027,11 @@
         </is>
       </c>
       <c r="D344" t="n">
-        <v>59952</v>
+        <v>112140</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>global gourmet  taco casserole</t>
+          <t>all in the kitchen  chili</t>
         </is>
       </c>
     </row>
@@ -9277,11 +9277,11 @@
         </is>
       </c>
       <c r="D354" t="n">
-        <v>99024</v>
+        <v>93249</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>smoked  salmon  cracker spread</t>
+          <t>grilled  ranch bread</t>
         </is>
       </c>
     </row>
@@ -9302,11 +9302,11 @@
         </is>
       </c>
       <c r="D355" t="n">
-        <v>107699</v>
+        <v>58224</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>deep fried dessert thingys</t>
+          <t>immoral  sandwich filling  loose meat</t>
         </is>
       </c>
     </row>
@@ -9327,11 +9327,11 @@
         </is>
       </c>
       <c r="D356" t="n">
-        <v>93249</v>
+        <v>99024</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>grilled  ranch bread</t>
+          <t>smoked  salmon  cracker spread</t>
         </is>
       </c>
     </row>
@@ -9377,11 +9377,11 @@
         </is>
       </c>
       <c r="D358" t="n">
-        <v>62368</v>
+        <v>54100</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>the best  chocolate chip cheesecake ever</t>
+          <t>grilled  venison burgers</t>
         </is>
       </c>
     </row>
@@ -9402,11 +9402,11 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>71635</v>
+        <v>33606</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>no bake  cookie crumble cheesecake</t>
+          <t>italian sandwich  pasta salad</t>
         </is>
       </c>
     </row>
@@ -9427,11 +9427,11 @@
         </is>
       </c>
       <c r="D360" t="n">
-        <v>54100</v>
+        <v>62368</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>grilled  venison burgers</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -9452,11 +9452,11 @@
         </is>
       </c>
       <c r="D361" t="n">
-        <v>99024</v>
+        <v>109439</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>smoked  salmon  cracker spread</t>
+          <t>berry  good sandwich spread</t>
         </is>
       </c>
     </row>
@@ -9527,11 +9527,11 @@
         </is>
       </c>
       <c r="D364" t="n">
-        <v>87098</v>
+        <v>44045</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>homemade  vegetable soup from a can</t>
+          <t>mennonite  corn fritters</t>
         </is>
       </c>
     </row>
@@ -9552,11 +9552,11 @@
         </is>
       </c>
       <c r="D365" t="n">
-        <v>44045</v>
+        <v>87098</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>mennonite  corn fritters</t>
+          <t>homemade  vegetable soup from a can</t>
         </is>
       </c>
     </row>
@@ -9577,11 +9577,11 @@
         </is>
       </c>
       <c r="D366" t="n">
-        <v>39959</v>
+        <v>112140</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>calm your nerves  tonic</t>
+          <t>all in the kitchen  chili</t>
         </is>
       </c>
     </row>
@@ -10252,11 +10252,11 @@
         </is>
       </c>
       <c r="D393" t="n">
-        <v>83133</v>
+        <v>87098</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>stove top  bbq  beef or pork ribs</t>
+          <t>homemade  vegetable soup from a can</t>
         </is>
       </c>
     </row>
@@ -10277,11 +10277,11 @@
         </is>
       </c>
       <c r="D394" t="n">
-        <v>87098</v>
+        <v>83133</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>homemade  vegetable soup from a can</t>
+          <t>stove top  bbq  beef or pork ribs</t>
         </is>
       </c>
     </row>
@@ -10327,11 +10327,11 @@
         </is>
       </c>
       <c r="D396" t="n">
-        <v>39959</v>
+        <v>112140</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>calm your nerves  tonic</t>
+          <t>all in the kitchen  chili</t>
         </is>
       </c>
     </row>
@@ -10377,11 +10377,11 @@
         </is>
       </c>
       <c r="D398" t="n">
-        <v>100870</v>
+        <v>25775</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>leftovers  spaghetti sauce</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -10402,11 +10402,11 @@
         </is>
       </c>
       <c r="D399" t="n">
-        <v>35173</v>
+        <v>100870</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>italian  gut busters</t>
+          <t>leftovers  spaghetti sauce</t>
         </is>
       </c>
     </row>
@@ -10427,11 +10427,11 @@
         </is>
       </c>
       <c r="D400" t="n">
-        <v>107699</v>
+        <v>35173</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>deep fried dessert thingys</t>
+          <t>italian  gut busters</t>
         </is>
       </c>
     </row>
@@ -10452,11 +10452,11 @@
         </is>
       </c>
       <c r="D401" t="n">
-        <v>35653</v>
+        <v>107699</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>make it your way  shortcakes</t>
+          <t>deep fried dessert thingys</t>
         </is>
       </c>
     </row>
@@ -10527,11 +10527,11 @@
         </is>
       </c>
       <c r="D404" t="n">
-        <v>25274</v>
+        <v>23933</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>aww  marinated olives</t>
+          <t>chinese  candy</t>
         </is>
       </c>
     </row>
@@ -11277,11 +11277,11 @@
         </is>
       </c>
       <c r="D434" t="n">
-        <v>25274</v>
+        <v>23933</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>aww  marinated olives</t>
+          <t>chinese  candy</t>
         </is>
       </c>
     </row>
@@ -11502,11 +11502,11 @@
         </is>
       </c>
       <c r="D443" t="n">
-        <v>58224</v>
+        <v>112140</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>immoral  sandwich filling  loose meat</t>
+          <t>all in the kitchen  chili</t>
         </is>
       </c>
     </row>
@@ -11577,11 +11577,11 @@
         </is>
       </c>
       <c r="D446" t="n">
-        <v>33606</v>
+        <v>58224</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>italian sandwich  pasta salad</t>
+          <t>immoral  sandwich filling  loose meat</t>
         </is>
       </c>
     </row>
@@ -12052,11 +12052,11 @@
         </is>
       </c>
       <c r="D465" t="n">
-        <v>52804</v>
+        <v>74805</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>jiffy  extra moist carrot cake</t>
+          <t>never weep  whipped cream</t>
         </is>
       </c>
     </row>
@@ -12077,11 +12077,11 @@
         </is>
       </c>
       <c r="D466" t="n">
-        <v>74805</v>
+        <v>52804</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
-          <t>never weep  whipped cream</t>
+          <t>jiffy  extra moist carrot cake</t>
         </is>
       </c>
     </row>
@@ -12227,11 +12227,11 @@
         </is>
       </c>
       <c r="D472" t="n">
-        <v>22123</v>
+        <v>63593</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
-          <t>i don t feel like cooking tonight  casserole</t>
+          <t>more  more    apple pear jigglers</t>
         </is>
       </c>
     </row>
@@ -12252,11 +12252,11 @@
         </is>
       </c>
       <c r="D473" t="n">
-        <v>58224</v>
+        <v>22123</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
-          <t>immoral  sandwich filling  loose meat</t>
+          <t>i don t feel like cooking tonight  casserole</t>
         </is>
       </c>
     </row>
@@ -12277,11 +12277,11 @@
         </is>
       </c>
       <c r="D474" t="n">
-        <v>39959</v>
+        <v>112140</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
-          <t>calm your nerves  tonic</t>
+          <t>all in the kitchen  chili</t>
         </is>
       </c>
     </row>
@@ -12302,11 +12302,11 @@
         </is>
       </c>
       <c r="D475" t="n">
-        <v>63593</v>
+        <v>39959</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
-          <t>more  more    apple pear jigglers</t>
+          <t>calm your nerves  tonic</t>
         </is>
       </c>
     </row>
@@ -12327,11 +12327,11 @@
         </is>
       </c>
       <c r="D476" t="n">
-        <v>33606</v>
+        <v>58224</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
-          <t>italian sandwich  pasta salad</t>
+          <t>immoral  sandwich filling  loose meat</t>
         </is>
       </c>
     </row>
@@ -12377,11 +12377,11 @@
         </is>
       </c>
       <c r="D478" t="n">
-        <v>35964</v>
+        <v>25775</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>rich  hot fudge cake</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -12402,11 +12402,11 @@
         </is>
       </c>
       <c r="D479" t="n">
-        <v>39959</v>
+        <v>35964</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>calm your nerves  tonic</t>
+          <t>rich  hot fudge cake</t>
         </is>
       </c>
     </row>
@@ -12427,11 +12427,11 @@
         </is>
       </c>
       <c r="D480" t="n">
-        <v>76808</v>
+        <v>39959</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
-          <t>cream  of spinach soup</t>
+          <t>calm your nerves  tonic</t>
         </is>
       </c>
     </row>
@@ -12452,11 +12452,11 @@
         </is>
       </c>
       <c r="D481" t="n">
-        <v>32169</v>
+        <v>76808</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t>make that chicken dance  salsa pasta</t>
+          <t>cream  of spinach soup</t>
         </is>
       </c>
     </row>
@@ -13002,11 +13002,11 @@
         </is>
       </c>
       <c r="D503" t="n">
-        <v>39363</v>
+        <v>75452</v>
       </c>
       <c r="E503" t="inlineStr">
         <is>
-          <t>the best  banana bread  or muffins</t>
+          <t>beat this  banana bread</t>
         </is>
       </c>
     </row>
@@ -13027,11 +13027,11 @@
         </is>
       </c>
       <c r="D504" t="n">
-        <v>75452</v>
+        <v>83062</v>
       </c>
       <c r="E504" t="inlineStr">
         <is>
-          <t>beat this  banana bread</t>
+          <t>spicy  banana bread</t>
         </is>
       </c>
     </row>
@@ -13052,11 +13052,11 @@
         </is>
       </c>
       <c r="D505" t="n">
-        <v>95926</v>
+        <v>39363</v>
       </c>
       <c r="E505" t="inlineStr">
         <is>
-          <t>say what   banana sandwich</t>
+          <t>the best  banana bread  or muffins</t>
         </is>
       </c>
     </row>
@@ -13077,11 +13077,11 @@
         </is>
       </c>
       <c r="D506" t="n">
-        <v>83062</v>
+        <v>95926</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
-          <t>spicy  banana bread</t>
+          <t>say what   banana sandwich</t>
         </is>
       </c>
     </row>
@@ -16052,11 +16052,11 @@
         </is>
       </c>
       <c r="D625" t="n">
-        <v>44123</v>
+        <v>59952</v>
       </c>
       <c r="E625" t="inlineStr">
         <is>
-          <t>george s at the cove  black bean soup</t>
+          <t>global gourmet  taco casserole</t>
         </is>
       </c>
     </row>
@@ -16077,11 +16077,11 @@
         </is>
       </c>
       <c r="D626" t="n">
-        <v>59952</v>
+        <v>44123</v>
       </c>
       <c r="E626" t="inlineStr">
         <is>
-          <t>global gourmet  taco casserole</t>
+          <t>george s at the cove  black bean soup</t>
         </is>
       </c>
     </row>
@@ -18002,11 +18002,11 @@
         </is>
       </c>
       <c r="D703" t="n">
-        <v>8559</v>
+        <v>38276</v>
       </c>
       <c r="E703" t="inlineStr">
         <is>
-          <t>chinese  chop suey</t>
+          <t>now and later  vegetarian empanadas</t>
         </is>
       </c>
     </row>
@@ -18052,11 +18052,11 @@
         </is>
       </c>
       <c r="D705" t="n">
-        <v>64045</v>
+        <v>67888</v>
       </c>
       <c r="E705" t="inlineStr">
         <is>
-          <t>some like it hot</t>
+          <t>backyard style  barbecued ribs</t>
         </is>
       </c>
     </row>
@@ -18077,11 +18077,11 @@
         </is>
       </c>
       <c r="D706" t="n">
-        <v>67888</v>
+        <v>64045</v>
       </c>
       <c r="E706" t="inlineStr">
         <is>
-          <t>backyard style  barbecued ribs</t>
+          <t>some like it hot</t>
         </is>
       </c>
     </row>
@@ -18402,11 +18402,11 @@
         </is>
       </c>
       <c r="D719" t="n">
-        <v>35653</v>
+        <v>63793</v>
       </c>
       <c r="E719" t="inlineStr">
         <is>
-          <t>make it your way  shortcakes</t>
+          <t>tide me over   indian chaat  simple veggie salad</t>
         </is>
       </c>
     </row>
@@ -18427,11 +18427,11 @@
         </is>
       </c>
       <c r="D720" t="n">
-        <v>63793</v>
+        <v>35653</v>
       </c>
       <c r="E720" t="inlineStr">
         <is>
-          <t>tide me over   indian chaat  simple veggie salad</t>
+          <t>make it your way  shortcakes</t>
         </is>
       </c>
     </row>
@@ -18452,11 +18452,11 @@
         </is>
       </c>
       <c r="D721" t="n">
-        <v>84797</v>
+        <v>108804</v>
       </c>
       <c r="E721" t="inlineStr">
         <is>
-          <t>love is in the air  beef fondue   sauces</t>
+          <t>put down your fork   tuna and bean salad</t>
         </is>
       </c>
     </row>
@@ -19002,11 +19002,11 @@
         </is>
       </c>
       <c r="D743" t="n">
-        <v>58224</v>
+        <v>42570</v>
       </c>
       <c r="E743" t="inlineStr">
         <is>
-          <t>immoral  sandwich filling  loose meat</t>
+          <t>pick me up  party chicken kabobs</t>
         </is>
       </c>
     </row>
@@ -19027,11 +19027,11 @@
         </is>
       </c>
       <c r="D744" t="n">
-        <v>42570</v>
+        <v>58224</v>
       </c>
       <c r="E744" t="inlineStr">
         <is>
-          <t>pick me up  party chicken kabobs</t>
+          <t>immoral  sandwich filling  loose meat</t>
         </is>
       </c>
     </row>
@@ -21452,11 +21452,11 @@
         </is>
       </c>
       <c r="D841" t="n">
-        <v>100870</v>
+        <v>25775</v>
       </c>
       <c r="E841" t="inlineStr">
         <is>
-          <t>leftovers  spaghetti sauce</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -22277,11 +22277,11 @@
         </is>
       </c>
       <c r="D874" t="n">
-        <v>95926</v>
+        <v>63793</v>
       </c>
       <c r="E874" t="inlineStr">
         <is>
-          <t>say what   banana sandwich</t>
+          <t>tide me over   indian chaat  simple veggie salad</t>
         </is>
       </c>
     </row>
@@ -22302,11 +22302,11 @@
         </is>
       </c>
       <c r="D875" t="n">
-        <v>63793</v>
+        <v>95926</v>
       </c>
       <c r="E875" t="inlineStr">
         <is>
-          <t>tide me over   indian chaat  simple veggie salad</t>
+          <t>say what   banana sandwich</t>
         </is>
       </c>
     </row>
@@ -22352,11 +22352,11 @@
         </is>
       </c>
       <c r="D877" t="n">
-        <v>35173</v>
+        <v>63793</v>
       </c>
       <c r="E877" t="inlineStr">
         <is>
-          <t>italian  gut busters</t>
+          <t>tide me over   indian chaat  simple veggie salad</t>
         </is>
       </c>
     </row>
@@ -22377,11 +22377,11 @@
         </is>
       </c>
       <c r="D878" t="n">
-        <v>39959</v>
+        <v>87098</v>
       </c>
       <c r="E878" t="inlineStr">
         <is>
-          <t>calm your nerves  tonic</t>
+          <t>homemade  vegetable soup from a can</t>
         </is>
       </c>
     </row>
@@ -22402,11 +22402,11 @@
         </is>
       </c>
       <c r="D879" t="n">
-        <v>95926</v>
+        <v>35173</v>
       </c>
       <c r="E879" t="inlineStr">
         <is>
-          <t>say what   banana sandwich</t>
+          <t>italian  gut busters</t>
         </is>
       </c>
     </row>
@@ -22427,11 +22427,11 @@
         </is>
       </c>
       <c r="D880" t="n">
-        <v>87098</v>
+        <v>39959</v>
       </c>
       <c r="E880" t="inlineStr">
         <is>
-          <t>homemade  vegetable soup from a can</t>
+          <t>calm your nerves  tonic</t>
         </is>
       </c>
     </row>
@@ -22452,11 +22452,11 @@
         </is>
       </c>
       <c r="D881" t="n">
-        <v>63793</v>
+        <v>95926</v>
       </c>
       <c r="E881" t="inlineStr">
         <is>
-          <t>tide me over   indian chaat  simple veggie salad</t>
+          <t>say what   banana sandwich</t>
         </is>
       </c>
     </row>
@@ -22552,11 +22552,11 @@
         </is>
       </c>
       <c r="D885" t="n">
-        <v>25274</v>
+        <v>30131</v>
       </c>
       <c r="E885" t="inlineStr">
         <is>
-          <t>aww  marinated olives</t>
+          <t>momma s special  marinade</t>
         </is>
       </c>
     </row>
@@ -22577,11 +22577,11 @@
         </is>
       </c>
       <c r="D886" t="n">
-        <v>30131</v>
+        <v>93249</v>
       </c>
       <c r="E886" t="inlineStr">
         <is>
-          <t>momma s special  marinade</t>
+          <t>grilled  ranch bread</t>
         </is>
       </c>
     </row>
@@ -23252,11 +23252,11 @@
         </is>
       </c>
       <c r="D913" t="n">
-        <v>111875</v>
+        <v>112959</v>
       </c>
       <c r="E913" t="inlineStr">
         <is>
-          <t>the elvis  smoothie</t>
+          <t>sour cream  avocado dip  vegan</t>
         </is>
       </c>
     </row>
@@ -23277,11 +23277,11 @@
         </is>
       </c>
       <c r="D914" t="n">
-        <v>112959</v>
+        <v>111875</v>
       </c>
       <c r="E914" t="inlineStr">
         <is>
-          <t>sour cream  avocado dip  vegan</t>
+          <t>the elvis  smoothie</t>
         </is>
       </c>
     </row>
@@ -23302,11 +23302,11 @@
         </is>
       </c>
       <c r="D915" t="n">
-        <v>25274</v>
+        <v>23850</v>
       </c>
       <c r="E915" t="inlineStr">
         <is>
-          <t>aww  marinated olives</t>
+          <t>cream  of cauliflower soup  vegan</t>
         </is>
       </c>
     </row>
@@ -23427,11 +23427,11 @@
         </is>
       </c>
       <c r="D920" t="n">
-        <v>25274</v>
+        <v>25775</v>
       </c>
       <c r="E920" t="inlineStr">
         <is>
-          <t>aww  marinated olives</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -23452,11 +23452,11 @@
         </is>
       </c>
       <c r="D921" t="n">
-        <v>25775</v>
+        <v>24701</v>
       </c>
       <c r="E921" t="inlineStr">
         <is>
-          <t>how i got my family to eat spinach  spinach casserole</t>
+          <t>cream  of spinach soup  vegan</t>
         </is>
       </c>
     </row>
@@ -24002,11 +24002,11 @@
         </is>
       </c>
       <c r="D943" t="n">
-        <v>64302</v>
+        <v>83133</v>
       </c>
       <c r="E943" t="inlineStr">
         <is>
-          <t>red  macaroni salad</t>
+          <t>stove top  bbq  beef or pork ribs</t>
         </is>
       </c>
     </row>
@@ -24027,11 +24027,11 @@
         </is>
       </c>
       <c r="D944" t="n">
-        <v>83133</v>
+        <v>64302</v>
       </c>
       <c r="E944" t="inlineStr">
         <is>
-          <t>stove top  bbq  beef or pork ribs</t>
+          <t>red  macaroni salad</t>
         </is>
       </c>
     </row>
@@ -24427,11 +24427,11 @@
         </is>
       </c>
       <c r="D960" t="n">
-        <v>60219</v>
+        <v>87098</v>
       </c>
       <c r="E960" t="inlineStr">
         <is>
-          <t>mexican pasta</t>
+          <t>homemade  vegetable soup from a can</t>
         </is>
       </c>
     </row>
@@ -24452,11 +24452,11 @@
         </is>
       </c>
       <c r="D961" t="n">
-        <v>32169</v>
+        <v>25775</v>
       </c>
       <c r="E961" t="inlineStr">
         <is>
-          <t>make that chicken dance  salsa pasta</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -25302,11 +25302,11 @@
         </is>
       </c>
       <c r="D995" t="n">
-        <v>32169</v>
+        <v>59952</v>
       </c>
       <c r="E995" t="inlineStr">
         <is>
-          <t>make that chicken dance  salsa pasta</t>
+          <t>global gourmet  taco casserole</t>
         </is>
       </c>
     </row>
@@ -25327,11 +25327,11 @@
         </is>
       </c>
       <c r="D996" t="n">
-        <v>59534</v>
+        <v>32169</v>
       </c>
       <c r="E996" t="inlineStr">
         <is>
-          <t>twisted american chop suey</t>
+          <t>make that chicken dance  salsa pasta</t>
         </is>
       </c>
     </row>
@@ -25377,11 +25377,11 @@
         </is>
       </c>
       <c r="D998" t="n">
-        <v>25775</v>
+        <v>59952</v>
       </c>
       <c r="E998" t="inlineStr">
         <is>
-          <t>how i got my family to eat spinach  spinach casserole</t>
+          <t>global gourmet  taco casserole</t>
         </is>
       </c>
     </row>
@@ -25402,11 +25402,11 @@
         </is>
       </c>
       <c r="D999" t="n">
-        <v>32169</v>
+        <v>25775</v>
       </c>
       <c r="E999" t="inlineStr">
         <is>
-          <t>make that chicken dance  salsa pasta</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -25427,11 +25427,11 @@
         </is>
       </c>
       <c r="D1000" t="n">
-        <v>59952</v>
+        <v>32169</v>
       </c>
       <c r="E1000" t="inlineStr">
         <is>
-          <t>global gourmet  taco casserole</t>
+          <t>make that chicken dance  salsa pasta</t>
         </is>
       </c>
     </row>
@@ -26227,11 +26227,11 @@
         </is>
       </c>
       <c r="D1032" t="n">
-        <v>59534</v>
+        <v>23850</v>
       </c>
       <c r="E1032" t="inlineStr">
         <is>
-          <t>twisted american chop suey</t>
+          <t>cream  of cauliflower soup  vegan</t>
         </is>
       </c>
     </row>
@@ -26252,11 +26252,11 @@
         </is>
       </c>
       <c r="D1033" t="n">
-        <v>23850</v>
+        <v>137739</v>
       </c>
       <c r="E1033" t="inlineStr">
         <is>
-          <t>cream  of cauliflower soup  vegan</t>
+          <t>arriba   baked winter squash mexican style</t>
         </is>
       </c>
     </row>
@@ -26277,11 +26277,11 @@
         </is>
       </c>
       <c r="D1034" t="n">
-        <v>137739</v>
+        <v>59534</v>
       </c>
       <c r="E1034" t="inlineStr">
         <is>
-          <t>arriba   baked winter squash mexican style</t>
+          <t>twisted american chop suey</t>
         </is>
       </c>
     </row>
@@ -26402,11 +26402,11 @@
         </is>
       </c>
       <c r="D1039" t="n">
-        <v>49262</v>
+        <v>137739</v>
       </c>
       <c r="E1039" t="inlineStr">
         <is>
-          <t>easiest ever  hollandaise sauce</t>
+          <t>arriba   baked winter squash mexican style</t>
         </is>
       </c>
     </row>
@@ -26427,11 +26427,11 @@
         </is>
       </c>
       <c r="D1040" t="n">
-        <v>23850</v>
+        <v>87098</v>
       </c>
       <c r="E1040" t="inlineStr">
         <is>
-          <t>cream  of cauliflower soup  vegan</t>
+          <t>homemade  vegetable soup from a can</t>
         </is>
       </c>
     </row>
@@ -26452,11 +26452,11 @@
         </is>
       </c>
       <c r="D1041" t="n">
-        <v>44123</v>
+        <v>23850</v>
       </c>
       <c r="E1041" t="inlineStr">
         <is>
-          <t>george s at the cove  black bean soup</t>
+          <t>cream  of cauliflower soup  vegan</t>
         </is>
       </c>
     </row>
@@ -27227,11 +27227,11 @@
         </is>
       </c>
       <c r="D1072" t="n">
-        <v>107229</v>
+        <v>83873</v>
       </c>
       <c r="E1072" t="inlineStr">
         <is>
-          <t>open sesame  noodles</t>
+          <t>crispy crunchy  chicken</t>
         </is>
       </c>
     </row>
@@ -27252,11 +27252,11 @@
         </is>
       </c>
       <c r="D1073" t="n">
-        <v>83873</v>
+        <v>107229</v>
       </c>
       <c r="E1073" t="inlineStr">
         <is>
-          <t>crispy crunchy  chicken</t>
+          <t>open sesame  noodles</t>
         </is>
       </c>
     </row>
@@ -27277,11 +27277,11 @@
         </is>
       </c>
       <c r="D1074" t="n">
-        <v>54272</v>
+        <v>63986</v>
       </c>
       <c r="E1074" t="inlineStr">
         <is>
-          <t>fool the meat eaters  chili</t>
+          <t>chicken lickin  good  pork chops</t>
         </is>
       </c>
     </row>
@@ -27302,11 +27302,11 @@
         </is>
       </c>
       <c r="D1075" t="n">
-        <v>63986</v>
+        <v>98930</v>
       </c>
       <c r="E1075" t="inlineStr">
         <is>
-          <t>chicken lickin  good  pork chops</t>
+          <t>steamed  chicken cutlets in packages</t>
         </is>
       </c>
     </row>
@@ -27327,11 +27327,11 @@
         </is>
       </c>
       <c r="D1076" t="n">
-        <v>98930</v>
+        <v>54272</v>
       </c>
       <c r="E1076" t="inlineStr">
         <is>
-          <t>steamed  chicken cutlets in packages</t>
+          <t>fool the meat eaters  chili</t>
         </is>
       </c>
     </row>
@@ -27352,11 +27352,11 @@
         </is>
       </c>
       <c r="D1077" t="n">
-        <v>42570</v>
+        <v>83873</v>
       </c>
       <c r="E1077" t="inlineStr">
         <is>
-          <t>pick me up  party chicken kabobs</t>
+          <t>crispy crunchy  chicken</t>
         </is>
       </c>
     </row>
@@ -27377,11 +27377,11 @@
         </is>
       </c>
       <c r="D1078" t="n">
-        <v>83873</v>
+        <v>42570</v>
       </c>
       <c r="E1078" t="inlineStr">
         <is>
-          <t>crispy crunchy  chicken</t>
+          <t>pick me up  party chicken kabobs</t>
         </is>
       </c>
     </row>
@@ -27452,11 +27452,11 @@
         </is>
       </c>
       <c r="D1081" t="n">
-        <v>44123</v>
+        <v>32169</v>
       </c>
       <c r="E1081" t="inlineStr">
         <is>
-          <t>george s at the cove  black bean soup</t>
+          <t>make that chicken dance  salsa pasta</t>
         </is>
       </c>
     </row>
@@ -28002,11 +28002,11 @@
         </is>
       </c>
       <c r="D1103" t="n">
-        <v>53402</v>
+        <v>32169</v>
       </c>
       <c r="E1103" t="inlineStr">
         <is>
-          <t>killer  lasagna</t>
+          <t>make that chicken dance  salsa pasta</t>
         </is>
       </c>
     </row>
@@ -28027,11 +28027,11 @@
         </is>
       </c>
       <c r="D1104" t="n">
-        <v>32169</v>
+        <v>53402</v>
       </c>
       <c r="E1104" t="inlineStr">
         <is>
-          <t>make that chicken dance  salsa pasta</t>
+          <t>killer  lasagna</t>
         </is>
       </c>
     </row>
@@ -28052,11 +28052,11 @@
         </is>
       </c>
       <c r="D1105" t="n">
-        <v>47366</v>
+        <v>94710</v>
       </c>
       <c r="E1105" t="inlineStr">
         <is>
-          <t>forgotten  minestrone</t>
+          <t>italian  fries</t>
         </is>
       </c>
     </row>
@@ -28077,11 +28077,11 @@
         </is>
       </c>
       <c r="D1106" t="n">
-        <v>94710</v>
+        <v>47366</v>
       </c>
       <c r="E1106" t="inlineStr">
         <is>
-          <t>italian  fries</t>
+          <t>forgotten  minestrone</t>
         </is>
       </c>
     </row>
@@ -30277,11 +30277,11 @@
         </is>
       </c>
       <c r="D1194" t="n">
-        <v>95926</v>
+        <v>30300</v>
       </c>
       <c r="E1194" t="inlineStr">
         <is>
-          <t>say what   banana sandwich</t>
+          <t>munch without guilt  tomatoes</t>
         </is>
       </c>
     </row>
@@ -30327,11 +30327,11 @@
         </is>
       </c>
       <c r="D1196" t="n">
-        <v>30300</v>
+        <v>95926</v>
       </c>
       <c r="E1196" t="inlineStr">
         <is>
-          <t>munch without guilt  tomatoes</t>
+          <t>say what   banana sandwich</t>
         </is>
       </c>
     </row>
@@ -30352,11 +30352,11 @@
         </is>
       </c>
       <c r="D1197" t="n">
-        <v>83062</v>
+        <v>30300</v>
       </c>
       <c r="E1197" t="inlineStr">
         <is>
-          <t>spicy  banana bread</t>
+          <t>munch without guilt  tomatoes</t>
         </is>
       </c>
     </row>
@@ -30377,11 +30377,11 @@
         </is>
       </c>
       <c r="D1198" t="n">
-        <v>30300</v>
+        <v>83062</v>
       </c>
       <c r="E1198" t="inlineStr">
         <is>
-          <t>munch without guilt  tomatoes</t>
+          <t>spicy  banana bread</t>
         </is>
       </c>
     </row>
@@ -30452,11 +30452,11 @@
         </is>
       </c>
       <c r="D1201" t="n">
-        <v>26995</v>
+        <v>75452</v>
       </c>
       <c r="E1201" t="inlineStr">
         <is>
-          <t>keep it going  german friendship cake</t>
+          <t>beat this  banana bread</t>
         </is>
       </c>
     </row>
@@ -31002,11 +31002,11 @@
         </is>
       </c>
       <c r="D1223" t="n">
-        <v>112140</v>
+        <v>59534</v>
       </c>
       <c r="E1223" t="inlineStr">
         <is>
-          <t>all in the kitchen  chili</t>
+          <t>twisted american chop suey</t>
         </is>
       </c>
     </row>
@@ -31027,11 +31027,11 @@
         </is>
       </c>
       <c r="D1224" t="n">
-        <v>59534</v>
+        <v>41756</v>
       </c>
       <c r="E1224" t="inlineStr">
         <is>
-          <t>twisted american chop suey</t>
+          <t>souper  easy sweet   sour meatballs</t>
         </is>
       </c>
     </row>
@@ -31052,11 +31052,11 @@
         </is>
       </c>
       <c r="D1225" t="n">
-        <v>41756</v>
+        <v>112140</v>
       </c>
       <c r="E1225" t="inlineStr">
         <is>
-          <t>souper  easy sweet   sour meatballs</t>
+          <t>all in the kitchen  chili</t>
         </is>
       </c>
     </row>
@@ -31327,11 +31327,11 @@
         </is>
       </c>
       <c r="D1236" t="n">
-        <v>95926</v>
+        <v>67664</v>
       </c>
       <c r="E1236" t="inlineStr">
         <is>
-          <t>say what   banana sandwich</t>
+          <t>healthy for them  yogurt popsicles</t>
         </is>
       </c>
     </row>
@@ -32352,11 +32352,11 @@
         </is>
       </c>
       <c r="D1277" t="n">
-        <v>42570</v>
+        <v>112959</v>
       </c>
       <c r="E1277" t="inlineStr">
         <is>
-          <t>pick me up  party chicken kabobs</t>
+          <t>sour cream  avocado dip  vegan</t>
         </is>
       </c>
     </row>
@@ -32377,11 +32377,11 @@
         </is>
       </c>
       <c r="D1278" t="n">
-        <v>112959</v>
+        <v>24701</v>
       </c>
       <c r="E1278" t="inlineStr">
         <is>
-          <t>sour cream  avocado dip  vegan</t>
+          <t>cream  of spinach soup  vegan</t>
         </is>
       </c>
     </row>
@@ -32402,11 +32402,11 @@
         </is>
       </c>
       <c r="D1279" t="n">
-        <v>54100</v>
+        <v>31490</v>
       </c>
       <c r="E1279" t="inlineStr">
         <is>
-          <t>grilled  venison burgers</t>
+          <t>a bit different  breakfast pizza</t>
         </is>
       </c>
     </row>
@@ -32427,11 +32427,11 @@
         </is>
       </c>
       <c r="D1280" t="n">
-        <v>54272</v>
+        <v>23850</v>
       </c>
       <c r="E1280" t="inlineStr">
         <is>
-          <t>fool the meat eaters  chili</t>
+          <t>cream  of cauliflower soup  vegan</t>
         </is>
       </c>
     </row>
@@ -32452,11 +32452,11 @@
         </is>
       </c>
       <c r="D1281" t="n">
-        <v>58224</v>
+        <v>42570</v>
       </c>
       <c r="E1281" t="inlineStr">
         <is>
-          <t>immoral  sandwich filling  loose meat</t>
+          <t>pick me up  party chicken kabobs</t>
         </is>
       </c>
     </row>
@@ -33752,11 +33752,11 @@
         </is>
       </c>
       <c r="D1333" t="n">
-        <v>38798</v>
+        <v>52804</v>
       </c>
       <c r="E1333" t="inlineStr">
         <is>
-          <t>i can t believe it s spinach</t>
+          <t>jiffy  extra moist carrot cake</t>
         </is>
       </c>
     </row>
@@ -33777,11 +33777,11 @@
         </is>
       </c>
       <c r="D1334" t="n">
-        <v>52804</v>
+        <v>26995</v>
       </c>
       <c r="E1334" t="inlineStr">
         <is>
-          <t>jiffy  extra moist carrot cake</t>
+          <t>keep it going  german friendship cake</t>
         </is>
       </c>
     </row>
@@ -33827,11 +33827,11 @@
         </is>
       </c>
       <c r="D1336" t="n">
-        <v>26995</v>
+        <v>27087</v>
       </c>
       <c r="E1336" t="inlineStr">
         <is>
-          <t>keep it going  german friendship cake</t>
+          <t>get the sensation  brownies</t>
         </is>
       </c>
     </row>
@@ -34052,11 +34052,11 @@
         </is>
       </c>
       <c r="D1345" t="n">
-        <v>93959</v>
+        <v>26835</v>
       </c>
       <c r="E1345" t="inlineStr">
         <is>
-          <t>i yam what i yam two  muffins</t>
+          <t>one bowl  perfect pound cake</t>
         </is>
       </c>
     </row>
@@ -34077,11 +34077,11 @@
         </is>
       </c>
       <c r="D1346" t="n">
-        <v>26835</v>
+        <v>75452</v>
       </c>
       <c r="E1346" t="inlineStr">
         <is>
-          <t>one bowl  perfect pound cake</t>
+          <t>beat this  banana bread</t>
         </is>
       </c>
     </row>
@@ -34377,11 +34377,11 @@
         </is>
       </c>
       <c r="D1358" t="n">
-        <v>26835</v>
+        <v>30300</v>
       </c>
       <c r="E1358" t="inlineStr">
         <is>
-          <t>one bowl  perfect pound cake</t>
+          <t>munch without guilt  tomatoes</t>
         </is>
       </c>
     </row>
@@ -34402,11 +34402,11 @@
         </is>
       </c>
       <c r="D1359" t="n">
-        <v>30300</v>
+        <v>26835</v>
       </c>
       <c r="E1359" t="inlineStr">
         <is>
-          <t>munch without guilt  tomatoes</t>
+          <t>one bowl  perfect pound cake</t>
         </is>
       </c>
     </row>
@@ -34427,11 +34427,11 @@
         </is>
       </c>
       <c r="D1360" t="n">
-        <v>71635</v>
+        <v>25775</v>
       </c>
       <c r="E1360" t="inlineStr">
         <is>
-          <t>no bake  cookie crumble cheesecake</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -34452,11 +34452,11 @@
         </is>
       </c>
       <c r="D1361" t="n">
-        <v>35653</v>
+        <v>71635</v>
       </c>
       <c r="E1361" t="inlineStr">
         <is>
-          <t>make it your way  shortcakes</t>
+          <t>no bake  cookie crumble cheesecake</t>
         </is>
       </c>
     </row>
@@ -35252,11 +35252,11 @@
         </is>
       </c>
       <c r="D1393" t="n">
-        <v>25274</v>
+        <v>24701</v>
       </c>
       <c r="E1393" t="inlineStr">
         <is>
-          <t>aww  marinated olives</t>
+          <t>cream  of spinach soup  vegan</t>
         </is>
       </c>
     </row>
@@ -35277,11 +35277,11 @@
         </is>
       </c>
       <c r="D1394" t="n">
-        <v>54272</v>
+        <v>25274</v>
       </c>
       <c r="E1394" t="inlineStr">
         <is>
-          <t>fool the meat eaters  chili</t>
+          <t>aww  marinated olives</t>
         </is>
       </c>
     </row>
@@ -35302,11 +35302,11 @@
         </is>
       </c>
       <c r="D1395" t="n">
-        <v>81185</v>
+        <v>54272</v>
       </c>
       <c r="E1395" t="inlineStr">
         <is>
-          <t>mock a mole   low fat guacamole</t>
+          <t>fool the meat eaters  chili</t>
         </is>
       </c>
     </row>
@@ -35327,11 +35327,11 @@
         </is>
       </c>
       <c r="D1396" t="n">
-        <v>24701</v>
+        <v>81185</v>
       </c>
       <c r="E1396" t="inlineStr">
         <is>
-          <t>cream  of spinach soup  vegan</t>
+          <t>mock a mole   low fat guacamole</t>
         </is>
       </c>
     </row>
@@ -35402,11 +35402,11 @@
         </is>
       </c>
       <c r="D1399" t="n">
-        <v>54272</v>
+        <v>23850</v>
       </c>
       <c r="E1399" t="inlineStr">
         <is>
-          <t>fool the meat eaters  chili</t>
+          <t>cream  of cauliflower soup  vegan</t>
         </is>
       </c>
     </row>
@@ -35427,11 +35427,11 @@
         </is>
       </c>
       <c r="D1400" t="n">
-        <v>23850</v>
+        <v>54272</v>
       </c>
       <c r="E1400" t="inlineStr">
         <is>
-          <t>cream  of cauliflower soup  vegan</t>
+          <t>fool the meat eaters  chili</t>
         </is>
       </c>
     </row>
@@ -35452,11 +35452,11 @@
         </is>
       </c>
       <c r="D1401" t="n">
-        <v>84797</v>
+        <v>25775</v>
       </c>
       <c r="E1401" t="inlineStr">
         <is>
-          <t>love is in the air  beef fondue   sauces</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -36327,11 +36327,11 @@
         </is>
       </c>
       <c r="D1436" t="n">
-        <v>42570</v>
+        <v>107699</v>
       </c>
       <c r="E1436" t="inlineStr">
         <is>
-          <t>pick me up  party chicken kabobs</t>
+          <t>deep fried dessert thingys</t>
         </is>
       </c>
     </row>
@@ -36352,11 +36352,11 @@
         </is>
       </c>
       <c r="D1437" t="n">
-        <v>35964</v>
+        <v>107699</v>
       </c>
       <c r="E1437" t="inlineStr">
         <is>
-          <t>rich  hot fudge cake</t>
+          <t>deep fried dessert thingys</t>
         </is>
       </c>
     </row>
@@ -36377,11 +36377,11 @@
         </is>
       </c>
       <c r="D1438" t="n">
-        <v>107699</v>
+        <v>35964</v>
       </c>
       <c r="E1438" t="inlineStr">
         <is>
-          <t>deep fried dessert thingys</t>
+          <t>rich  hot fudge cake</t>
         </is>
       </c>
     </row>
@@ -37352,11 +37352,11 @@
         </is>
       </c>
       <c r="D1477" t="n">
-        <v>52804</v>
+        <v>107699</v>
       </c>
       <c r="E1477" t="inlineStr">
         <is>
-          <t>jiffy  extra moist carrot cake</t>
+          <t>deep fried dessert thingys</t>
         </is>
       </c>
     </row>
@@ -37377,11 +37377,11 @@
         </is>
       </c>
       <c r="D1478" t="n">
-        <v>107699</v>
+        <v>52804</v>
       </c>
       <c r="E1478" t="inlineStr">
         <is>
-          <t>deep fried dessert thingys</t>
+          <t>jiffy  extra moist carrot cake</t>
         </is>
       </c>
     </row>
@@ -38027,11 +38027,11 @@
         </is>
       </c>
       <c r="D1504" t="n">
-        <v>35964</v>
+        <v>62368</v>
       </c>
       <c r="E1504" t="inlineStr">
         <is>
-          <t>rich  hot fudge cake</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -38052,11 +38052,11 @@
         </is>
       </c>
       <c r="D1505" t="n">
-        <v>62368</v>
+        <v>38276</v>
       </c>
       <c r="E1505" t="inlineStr">
         <is>
-          <t>the best  chocolate chip cheesecake ever</t>
+          <t>now and later  vegetarian empanadas</t>
         </is>
       </c>
     </row>
@@ -38077,11 +38077,11 @@
         </is>
       </c>
       <c r="D1506" t="n">
-        <v>39363</v>
+        <v>35653</v>
       </c>
       <c r="E1506" t="inlineStr">
         <is>
-          <t>the best  banana bread  or muffins</t>
+          <t>make it your way  shortcakes</t>
         </is>
       </c>
     </row>
@@ -38352,11 +38352,11 @@
         </is>
       </c>
       <c r="D1517" t="n">
-        <v>71635</v>
+        <v>71457</v>
       </c>
       <c r="E1517" t="inlineStr">
         <is>
-          <t>no bake  cookie crumble cheesecake</t>
+          <t>rise and shine  german fruit pancake</t>
         </is>
       </c>
     </row>
@@ -38377,11 +38377,11 @@
         </is>
       </c>
       <c r="D1518" t="n">
-        <v>62368</v>
+        <v>71635</v>
       </c>
       <c r="E1518" t="inlineStr">
         <is>
-          <t>the best  chocolate chip cheesecake ever</t>
+          <t>no bake  cookie crumble cheesecake</t>
         </is>
       </c>
     </row>
@@ -38402,11 +38402,11 @@
         </is>
       </c>
       <c r="D1519" t="n">
-        <v>71457</v>
+        <v>62368</v>
       </c>
       <c r="E1519" t="inlineStr">
         <is>
-          <t>rise and shine  german fruit pancake</t>
+          <t>the best  chocolate chip cheesecake ever</t>
         </is>
       </c>
     </row>
@@ -39252,11 +39252,11 @@
         </is>
       </c>
       <c r="D1553" t="n">
-        <v>25274</v>
+        <v>60219</v>
       </c>
       <c r="E1553" t="inlineStr">
         <is>
-          <t>aww  marinated olives</t>
+          <t>mexican pasta</t>
         </is>
       </c>
     </row>
@@ -39277,11 +39277,11 @@
         </is>
       </c>
       <c r="D1554" t="n">
-        <v>60219</v>
+        <v>25274</v>
       </c>
       <c r="E1554" t="inlineStr">
         <is>
-          <t>mexican pasta</t>
+          <t>aww  marinated olives</t>
         </is>
       </c>
     </row>
@@ -39302,11 +39302,11 @@
         </is>
       </c>
       <c r="D1555" t="n">
-        <v>54100</v>
+        <v>32169</v>
       </c>
       <c r="E1555" t="inlineStr">
         <is>
-          <t>grilled  venison burgers</t>
+          <t>make that chicken dance  salsa pasta</t>
         </is>
       </c>
     </row>
@@ -39327,11 +39327,11 @@
         </is>
       </c>
       <c r="D1556" t="n">
-        <v>107229</v>
+        <v>54100</v>
       </c>
       <c r="E1556" t="inlineStr">
         <is>
-          <t>open sesame  noodles</t>
+          <t>grilled  venison burgers</t>
         </is>
       </c>
     </row>
@@ -39402,11 +39402,11 @@
         </is>
       </c>
       <c r="D1559" t="n">
-        <v>49262</v>
+        <v>32169</v>
       </c>
       <c r="E1559" t="inlineStr">
         <is>
-          <t>easiest ever  hollandaise sauce</t>
+          <t>make that chicken dance  salsa pasta</t>
         </is>
       </c>
     </row>
@@ -39427,11 +39427,11 @@
         </is>
       </c>
       <c r="D1560" t="n">
-        <v>107229</v>
+        <v>49262</v>
       </c>
       <c r="E1560" t="inlineStr">
         <is>
-          <t>open sesame  noodles</t>
+          <t>easiest ever  hollandaise sauce</t>
         </is>
       </c>
     </row>
@@ -39452,11 +39452,11 @@
         </is>
       </c>
       <c r="D1561" t="n">
-        <v>32169</v>
+        <v>107229</v>
       </c>
       <c r="E1561" t="inlineStr">
         <is>
-          <t>make that chicken dance  salsa pasta</t>
+          <t>open sesame  noodles</t>
         </is>
       </c>
     </row>
@@ -41377,11 +41377,11 @@
         </is>
       </c>
       <c r="D1638" t="n">
-        <v>27087</v>
+        <v>39947</v>
       </c>
       <c r="E1638" t="inlineStr">
         <is>
-          <t>get the sensation  brownies</t>
+          <t>sugared grapes</t>
         </is>
       </c>
     </row>
@@ -41402,11 +41402,11 @@
         </is>
       </c>
       <c r="D1639" t="n">
-        <v>39947</v>
+        <v>27087</v>
       </c>
       <c r="E1639" t="inlineStr">
         <is>
-          <t>sugared grapes</t>
+          <t>get the sensation  brownies</t>
         </is>
       </c>
     </row>
@@ -42252,11 +42252,11 @@
         </is>
       </c>
       <c r="D1673" t="n">
-        <v>103948</v>
+        <v>31490</v>
       </c>
       <c r="E1673" t="inlineStr">
         <is>
-          <t>smells like sunday  chicken fricassee with meatballs</t>
+          <t>a bit different  breakfast pizza</t>
         </is>
       </c>
     </row>
@@ -42277,11 +42277,11 @@
         </is>
       </c>
       <c r="D1674" t="n">
-        <v>39363</v>
+        <v>103948</v>
       </c>
       <c r="E1674" t="inlineStr">
         <is>
-          <t>the best  banana bread  or muffins</t>
+          <t>smells like sunday  chicken fricassee with meatballs</t>
         </is>
       </c>
     </row>
@@ -42302,11 +42302,11 @@
         </is>
       </c>
       <c r="D1675" t="n">
-        <v>31490</v>
+        <v>25775</v>
       </c>
       <c r="E1675" t="inlineStr">
         <is>
-          <t>a bit different  breakfast pizza</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -42327,11 +42327,11 @@
         </is>
       </c>
       <c r="D1676" t="n">
-        <v>25775</v>
+        <v>39363</v>
       </c>
       <c r="E1676" t="inlineStr">
         <is>
-          <t>how i got my family to eat spinach  spinach casserole</t>
+          <t>the best  banana bread  or muffins</t>
         </is>
       </c>
     </row>
@@ -42377,11 +42377,11 @@
         </is>
       </c>
       <c r="D1678" t="n">
-        <v>22526</v>
+        <v>31490</v>
       </c>
       <c r="E1678" t="inlineStr">
         <is>
-          <t>land of nod  cinnamon buns</t>
+          <t>a bit different  breakfast pizza</t>
         </is>
       </c>
     </row>
@@ -42402,11 +42402,11 @@
         </is>
       </c>
       <c r="D1679" t="n">
-        <v>71457</v>
+        <v>22526</v>
       </c>
       <c r="E1679" t="inlineStr">
         <is>
-          <t>rise and shine  german fruit pancake</t>
+          <t>land of nod  cinnamon buns</t>
         </is>
       </c>
     </row>
@@ -42427,11 +42427,11 @@
         </is>
       </c>
       <c r="D1680" t="n">
-        <v>107229</v>
+        <v>71457</v>
       </c>
       <c r="E1680" t="inlineStr">
         <is>
-          <t>open sesame  noodles</t>
+          <t>rise and shine  german fruit pancake</t>
         </is>
       </c>
     </row>
@@ -42452,11 +42452,11 @@
         </is>
       </c>
       <c r="D1681" t="n">
-        <v>64045</v>
+        <v>25775</v>
       </c>
       <c r="E1681" t="inlineStr">
         <is>
-          <t>some like it hot</t>
+          <t>how i got my family to eat spinach  spinach casserole</t>
         </is>
       </c>
     </row>
@@ -43277,11 +43277,11 @@
         </is>
       </c>
       <c r="D1714" t="n">
-        <v>27087</v>
+        <v>112959</v>
       </c>
       <c r="E1714" t="inlineStr">
         <is>
-          <t>get the sensation  brownies</t>
+          <t>sour cream  avocado dip  vegan</t>
         </is>
       </c>
     </row>
@@ -43302,11 +43302,11 @@
         </is>
       </c>
       <c r="D1715" t="n">
-        <v>112959</v>
+        <v>27087</v>
       </c>
       <c r="E1715" t="inlineStr">
         <is>
-          <t>sour cream  avocado dip  vegan</t>
+          <t>get the sensation  brownies</t>
         </is>
       </c>
     </row>
@@ -43402,11 +43402,11 @@
         </is>
       </c>
       <c r="D1719" t="n">
-        <v>54272</v>
+        <v>23850</v>
       </c>
       <c r="E1719" t="inlineStr">
         <is>
-          <t>fool the meat eaters  chili</t>
+          <t>cream  of cauliflower soup  vegan</t>
         </is>
       </c>
     </row>
@@ -43427,11 +43427,11 @@
         </is>
       </c>
       <c r="D1720" t="n">
-        <v>42570</v>
+        <v>54272</v>
       </c>
       <c r="E1720" t="inlineStr">
         <is>
-          <t>pick me up  party chicken kabobs</t>
+          <t>fool the meat eaters  chili</t>
         </is>
       </c>
     </row>
@@ -43452,11 +43452,11 @@
         </is>
       </c>
       <c r="D1721" t="n">
-        <v>8559</v>
+        <v>42570</v>
       </c>
       <c r="E1721" t="inlineStr">
         <is>
-          <t>chinese  chop suey</t>
+          <t>pick me up  party chicken kabobs</t>
         </is>
       </c>
     </row>
@@ -44402,11 +44402,11 @@
         </is>
       </c>
       <c r="D1759" t="n">
-        <v>33606</v>
+        <v>87098</v>
       </c>
       <c r="E1759" t="inlineStr">
         <is>
-          <t>italian sandwich  pasta salad</t>
+          <t>homemade  vegetable soup from a can</t>
         </is>
       </c>
     </row>
@@ -44427,11 +44427,11 @@
         </is>
       </c>
       <c r="D1760" t="n">
-        <v>32169</v>
+        <v>33606</v>
       </c>
       <c r="E1760" t="inlineStr">
         <is>
-          <t>make that chicken dance  salsa pasta</t>
+          <t>italian sandwich  pasta salad</t>
         </is>
       </c>
     </row>
@@ -44452,11 +44452,11 @@
         </is>
       </c>
       <c r="D1761" t="n">
-        <v>90921</v>
+        <v>32169</v>
       </c>
       <c r="E1761" t="inlineStr">
         <is>
-          <t>i stole the idea from mirj  sesame noodles</t>
+          <t>make that chicken dance  salsa pasta</t>
         </is>
       </c>
     </row>

</xml_diff>